<commit_message>
Initial release: Complete welfare assessment pipeline for Atlantic salmon
Includes comprehensive analysis modules for:
- DNA damage assessment (telomere length, methylation, oxidative damage)
- Oxidative stress quantification
- Non-linear growth modeling
- Survival analysis
- Thermoregulatory behavior analysis
- Cumulative welfare assessment

Complete with documentation, data files, and automated analysis scripts.
</commit_message>
<xml_diff>
--- a/Data/Growth/Growth_SD.xlsx
+++ b/Data/Growth/Growth_SD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natal\Dropbox\One_drive\Documentos\Paper_Long_welfare\Growth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5ab59e229eea4afa/Welfare_S.salar_2025/Data/Growth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBA5377-6C47-4187-8D67-4CED3F9AEDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8EBA5377-6C47-4187-8D67-4CED3F9AEDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC27ABA1-C1A3-48CF-8D46-762E35724141}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6BDDF53-3D3A-49BF-AEF7-AB1867111480}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6BDDF53-3D3A-49BF-AEF7-AB1867111480}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:D163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +468,7 @@
         <v>0.13</v>
       </c>
       <c r="D2">
-        <v>4.3034869582699982E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -482,7 +482,7 @@
         <v>0.13700000000000001</v>
       </c>
       <c r="D3">
-        <v>1.2767145334803717E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="D4">
-        <v>6.5368187981616879E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -510,7 +510,7 @@
         <v>0.11700000000000001</v>
       </c>
       <c r="D5">
-        <v>2.251666049839534E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="D6">
-        <v>3.1575306807693854E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="D7">
-        <v>1.2529964086141652E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
         <v>0.112</v>
       </c>
       <c r="D8">
-        <v>7.8172885324772304E-2</v>
+        <v>7.8E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,7 +566,7 @@
         <v>0.14299999999999999</v>
       </c>
       <c r="D9">
-        <v>5.550675634551161E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="D10">
-        <v>3.0413812651491078E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -594,7 +594,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="D11">
-        <v>6.6700824582609161E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
         <v>0.23</v>
       </c>
       <c r="D12">
-        <v>2.4515301344262535E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
         <v>0.31</v>
       </c>
       <c r="D13">
-        <v>6.872408602520666E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>0.15</v>
       </c>
       <c r="D14">
-        <v>3.7643060449437354E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
         <v>0.247</v>
       </c>
       <c r="D15">
-        <v>0.1034069630150697</v>
+        <v>0.10299999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
         <v>0.152</v>
       </c>
       <c r="D16">
-        <v>1.7349351572897465E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>0.28799999999999998</v>
       </c>
       <c r="D17">
-        <v>0.13617635624439342</v>
+        <v>0.13600000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>0.20300000000000001</v>
       </c>
       <c r="D18">
-        <v>4.838388161361188E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>0.32900000000000001</v>
       </c>
       <c r="D19">
-        <v>7.5498344352707566E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
         <v>0.158</v>
       </c>
       <c r="D20">
-        <v>2.3643180835073569E-2</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D21">
-        <v>0.11171839597845996</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>0.254</v>
       </c>
       <c r="D22">
-        <v>9.7534609242053052E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
         <v>0.26200000000000001</v>
       </c>
       <c r="D23">
-        <v>0.19410564133996722</v>
+        <v>0.19400000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>0.48</v>
       </c>
       <c r="D24">
-        <v>0.32258487255294538</v>
+        <v>0.32300000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -790,7 +790,7 @@
         <v>0.36199999999999999</v>
       </c>
       <c r="D25">
-        <v>0.16281277591147447</v>
+        <v>0.16300000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
         <v>0.34100000000000003</v>
       </c>
       <c r="D26">
-        <v>0.36927361129655617</v>
+        <v>0.36899999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,7 +818,7 @@
         <v>0.308</v>
       </c>
       <c r="D27">
-        <v>7.4478184725461694E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
         <v>0.23699999999999999</v>
       </c>
       <c r="D28">
-        <v>4.5923850012820136E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
         <v>0.36399999999999999</v>
       </c>
       <c r="D29">
-        <v>0.36307988101793809</v>
+        <v>0.36299999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>0.19</v>
       </c>
       <c r="D30">
-        <v>9.7072138124180654E-2</v>
+        <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -874,7 +874,7 @@
         <v>0.52200000000000002</v>
       </c>
       <c r="D31">
-        <v>0.37594813472073513</v>
+        <v>0.376</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -888,7 +888,7 @@
         <v>0.47099999999999997</v>
       </c>
       <c r="D32">
-        <v>0.21151595684486793</v>
+        <v>0.21199999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
         <v>0.25600000000000001</v>
       </c>
       <c r="D33">
-        <v>0.18796010214936573</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -916,7 +916,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="D34">
-        <v>9.4503968170654054E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -930,7 +930,7 @@
         <v>0.44900000000000001</v>
       </c>
       <c r="D35">
-        <v>0.34890113212771323</v>
+        <v>0.34899999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
         <v>0.42399999999999999</v>
       </c>
       <c r="D36">
-        <v>0.11214722466472367</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -958,7 +958,7 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="D37">
-        <v>0.39428542960652257</v>
+        <v>0.39400000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -972,7 +972,7 @@
         <v>0.627</v>
       </c>
       <c r="D38">
-        <v>0.13104579352272283</v>
+        <v>0.13100000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -986,7 +986,7 @@
         <v>0.61399999999999999</v>
       </c>
       <c r="D39">
-        <v>0.52182755772381351</v>
+        <v>0.52200000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1000,7 +1000,7 @@
         <v>0.65700000000000003</v>
       </c>
       <c r="D40">
-        <v>0.54819066026337959</v>
+        <v>0.54800000000000004</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>0.86499999999999999</v>
       </c>
       <c r="D41">
-        <v>0.49672527618392853</v>
+        <v>0.497</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1028,7 +1028,7 @@
         <v>0.74099999999999999</v>
       </c>
       <c r="D42">
-        <v>0.35085609585697647</v>
+        <v>0.35099999999999998</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>0.56399999999999995</v>
       </c>
       <c r="D43">
-        <v>0.26366455962074226</v>
+        <v>0.26400000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1056,7 +1056,7 @@
         <v>0.60199999999999998</v>
       </c>
       <c r="D44">
-        <v>0.39024735745421762</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1070,7 +1070,7 @@
         <v>0.80300000000000005</v>
       </c>
       <c r="D45">
-        <v>0.25471356461719924</v>
+        <v>0.255</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1084,7 +1084,7 @@
         <v>0.6</v>
       </c>
       <c r="D46">
-        <v>0.14742116537322547</v>
+        <v>0.14699999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,7 +1098,7 @@
         <v>0.879</v>
       </c>
       <c r="D47">
-        <v>0.68903047828089581</v>
+        <v>0.68899999999999995</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
         <v>0.76600000000000001</v>
       </c>
       <c r="D48">
-        <v>0.43455839653606948</v>
+        <v>0.435</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>0.995</v>
       </c>
       <c r="D49">
-        <v>1.1579080274356852</v>
+        <v>1.1579999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
         <v>0.873</v>
       </c>
       <c r="D50">
-        <v>0.49021321891601399</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
         <v>0.66</v>
       </c>
       <c r="D51">
-        <v>0.31294088898704164</v>
+        <v>0.313</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
         <v>0.96499999999999997</v>
       </c>
       <c r="D52">
-        <v>0.18723247581549457</v>
+        <v>0.187</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>0.88500000000000001</v>
       </c>
       <c r="D53">
-        <v>0.2987892233665736</v>
+        <v>0.29899999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>0.94899999999999995</v>
       </c>
       <c r="D54">
-        <v>0.50997745048188148</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
         <v>0.83</v>
       </c>
       <c r="D55">
-        <v>0.45571153156355393</v>
+        <v>0.45600000000000002</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,7 +1224,7 @@
         <v>0.82799999999999996</v>
       </c>
       <c r="D56">
-        <v>0.30350617786134121</v>
+        <v>0.30399999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1238,7 +1238,7 @@
         <v>1.081</v>
       </c>
       <c r="D57">
-        <v>0.2503357745109559</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
         <v>1.0880000000000001</v>
       </c>
       <c r="D58">
-        <v>0.41930060815600995</v>
+        <v>0.41899999999999998</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,7 +1266,7 @@
         <v>1.6080000000000001</v>
       </c>
       <c r="D59">
-        <v>0.89071712681411941</v>
+        <v>0.89100000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,7 +1280,7 @@
         <v>1.2729999999999999</v>
       </c>
       <c r="D60">
-        <v>0.58041278414590358</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
         <v>1.448</v>
       </c>
       <c r="D61">
-        <v>0.33616662535117808</v>
+        <v>0.33600000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1308,7 +1308,7 @@
         <v>1.163</v>
       </c>
       <c r="D62">
-        <v>0.46829584666106122</v>
+        <v>0.46800000000000003</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1322,7 +1322,7 @@
         <v>1.4990000000000001</v>
       </c>
       <c r="D63">
-        <v>0.80014186242190843</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,7 +1336,7 @@
         <v>1.673</v>
       </c>
       <c r="D64">
-        <v>0.39790576773904557</v>
+        <v>0.39800000000000002</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,7 +1350,7 @@
         <v>1.3720000000000001</v>
       </c>
       <c r="D65">
-        <v>0.17782294565100268</v>
+        <v>0.17799999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1364,7 +1364,7 @@
         <v>1.522</v>
       </c>
       <c r="D66">
-        <v>0.82657546539925808</v>
+        <v>0.82699999999999996</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1378,7 +1378,7 @@
         <v>1.198</v>
       </c>
       <c r="D67">
-        <v>0.35867673467901462</v>
+        <v>0.35899999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>1.681</v>
       </c>
       <c r="D68">
-        <v>0.7957656690257493</v>
+        <v>0.79600000000000004</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
         <v>1.861</v>
       </c>
       <c r="D69">
-        <v>0.6320830641616656</v>
+        <v>0.63200000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>1.7549999999999999</v>
       </c>
       <c r="D70">
-        <v>0.9582003965768332</v>
+        <v>0.95799999999999996</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1434,7 +1434,7 @@
         <v>1.61</v>
       </c>
       <c r="D71">
-        <v>1.0242812113867947</v>
+        <v>1.024</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>1.738</v>
       </c>
       <c r="D72">
-        <v>0.78836730018437462</v>
+        <v>0.78800000000000003</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
         <v>1.839</v>
       </c>
       <c r="D73">
-        <v>0.34913750872686333</v>
+        <v>0.34899999999999998</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1476,7 +1476,7 @@
         <v>2.1259999999999999</v>
       </c>
       <c r="D74">
-        <v>0.76045578438197148</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1490,7 +1490,7 @@
         <v>1.8660000000000001</v>
       </c>
       <c r="D75">
-        <v>0.60888997364055752</v>
+        <v>0.60899999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>1.992</v>
       </c>
       <c r="D76">
-        <v>0.57675037928032669</v>
+        <v>0.57699999999999996</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
         <v>1.9159999999999999</v>
       </c>
       <c r="D77">
-        <v>1.0509638433362005</v>
+        <v>1.0509999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1532,7 +1532,7 @@
         <v>2.0990000000000002</v>
       </c>
       <c r="D78">
-        <v>1.3386739707636055</v>
+        <v>1.339</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1546,7 +1546,7 @@
         <v>1.849</v>
       </c>
       <c r="D79">
-        <v>0.37352509955824836</v>
+        <v>0.374</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1560,7 +1560,7 @@
         <v>2.0169999999999999</v>
       </c>
       <c r="D80">
-        <v>0.6075154319027628</v>
+        <v>0.60799999999999998</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1574,7 +1574,7 @@
         <v>1.9730000000000001</v>
       </c>
       <c r="D81">
-        <v>0.98127875754038441</v>
+        <v>0.98099999999999998</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
         <v>2.0649999999999999</v>
       </c>
       <c r="D82">
-        <v>0.6266793438434044</v>
+        <v>0.627</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1602,7 +1602,7 @@
         <v>0.105</v>
       </c>
       <c r="D83">
-        <v>2.3259406699226087E-2</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1616,7 +1616,7 @@
         <v>0.13400000000000001</v>
       </c>
       <c r="D84">
-        <v>1.7320508075688791E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1630,7 +1630,7 @@
         <v>0.129</v>
       </c>
       <c r="D85">
-        <v>1.2124355652982137E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,7 +1644,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="D86">
-        <v>6.2217360921209032E-2</v>
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1658,7 +1658,7 @@
         <v>7.8E-2</v>
       </c>
       <c r="D87">
-        <v>3.3286633954186497E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1672,7 +1672,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="D88">
-        <v>2.5119713374160899E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="D89">
-        <v>1.4730919862656271E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1700,7 +1700,7 @@
         <v>0.1</v>
       </c>
       <c r="D90">
-        <v>1.2124355652982166E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1714,7 +1714,7 @@
         <v>0.16300000000000001</v>
       </c>
       <c r="D91">
-        <v>1.5716233645501721E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1728,7 +1728,7 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="D92">
-        <v>4.3714985988788785E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1742,7 +1742,7 @@
         <v>0.21</v>
       </c>
       <c r="D93">
-        <v>0.15629139451678078</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
         <v>0.248</v>
       </c>
       <c r="D94">
-        <v>8.4124907132192422E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -1770,7 +1770,7 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="D95">
-        <v>4.4799553569204176E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -1784,7 +1784,7 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="D96">
-        <v>0.15710187777362813</v>
+        <v>0.157</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -1798,7 +1798,7 @@
         <v>0.28399999999999997</v>
       </c>
       <c r="D97">
-        <v>7.7311060010841898E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -1812,7 +1812,7 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="D98">
-        <v>6.0024994793835634E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -1826,7 +1826,7 @@
         <v>0.33</v>
       </c>
       <c r="D99">
-        <v>0.24488160404571022</v>
+        <v>0.245</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="D100">
-        <v>3.8935844667863526E-2</v>
+        <v>3.9E-2</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1854,7 +1854,7 @@
         <v>0.192</v>
       </c>
       <c r="D101">
-        <v>4.5508241011930975E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1868,7 +1868,7 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="D102">
-        <v>0.15096025967121288</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1882,7 +1882,7 @@
         <v>0.26900000000000002</v>
       </c>
       <c r="D103">
-        <v>4.5705579528105687E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -1896,7 +1896,7 @@
         <v>0.23100000000000001</v>
       </c>
       <c r="D104">
-        <v>0.10558882516630248</v>
+        <v>0.106</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
         <v>0.33800000000000002</v>
       </c>
       <c r="D105">
-        <v>8.8898818889791745E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -1924,7 +1924,7 @@
         <v>0.245</v>
       </c>
       <c r="D106">
-        <v>0.11860860002546195</v>
+        <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -1938,7 +1938,7 @@
         <v>0.35399999999999998</v>
       </c>
       <c r="D107">
-        <v>7.4986665481270851E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1952,7 +1952,7 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="D108">
-        <v>5.4286278192559781E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
         <v>0.36299999999999999</v>
       </c>
       <c r="D109">
-        <v>0.14126924647636513</v>
+        <v>0.14099999999999999</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -1980,7 +1980,7 @@
         <v>0.35499999999999998</v>
       </c>
       <c r="D110">
-        <v>0.15156186855538573</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -1994,7 +1994,7 @@
         <v>0.375</v>
       </c>
       <c r="D111">
-        <v>0.12011244731500571</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2008,7 +2008,7 @@
         <v>0.38500000000000001</v>
       </c>
       <c r="D112">
-        <v>6.7134193969988279E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2022,7 +2022,7 @@
         <v>0.495</v>
       </c>
       <c r="D113">
-        <v>9.2065194291871447E-2</v>
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2036,7 +2036,7 @@
         <v>0.318</v>
       </c>
       <c r="D114">
-        <v>9.1065910196955827E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2050,7 +2050,7 @@
         <v>0.53800000000000003</v>
       </c>
       <c r="D115">
-        <v>0.1515948547939541</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2064,7 +2064,7 @@
         <v>0.48699999999999999</v>
       </c>
       <c r="D116">
-        <v>0.10886229834061011</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2078,7 +2078,7 @@
         <v>0.48199999999999998</v>
       </c>
       <c r="D117">
-        <v>0.18464289859076607</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2092,7 +2092,7 @@
         <v>0.59</v>
       </c>
       <c r="D118">
-        <v>0.30592319297496884</v>
+        <v>0.30599999999999999</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2106,7 +2106,7 @@
         <v>0.57899999999999996</v>
       </c>
       <c r="D119">
-        <v>7.3505101863747771E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2120,7 +2120,7 @@
         <v>0.60799999999999998</v>
       </c>
       <c r="D120">
-        <v>8.9716219269426759E-2</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2134,7 +2134,7 @@
         <v>0.78600000000000003</v>
       </c>
       <c r="D121">
-        <v>0.64598529395025683</v>
+        <v>0.64600000000000002</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2148,7 +2148,7 @@
         <v>0.80130000000000001</v>
       </c>
       <c r="D122">
-        <v>0.31215343983368188</v>
+        <v>0.312</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2162,7 +2162,7 @@
         <v>0.91399999999999992</v>
       </c>
       <c r="D123">
-        <v>9.8147847658519666E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
         <v>0.93100000000000005</v>
       </c>
       <c r="D124">
-        <v>3.1320919526731682E-2</v>
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2190,7 +2190,7 @@
         <v>1.004</v>
       </c>
       <c r="D125">
-        <v>0.35724081513735267</v>
+        <v>0.35699999999999998</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2204,7 +2204,7 @@
         <v>1.1670000000000003</v>
       </c>
       <c r="D126">
-        <v>0.70662649256874066</v>
+        <v>0.70699999999999996</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2218,7 +2218,7 @@
         <v>0.996</v>
       </c>
       <c r="D127">
-        <v>0.34998999985713874</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2232,7 +2232,7 @@
         <v>1.2370000000000001</v>
       </c>
       <c r="D128">
-        <v>0.10412972678346955</v>
+        <v>0.104</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -2246,7 +2246,7 @@
         <v>1.3510000000000002</v>
       </c>
       <c r="D129">
-        <v>0.44116663518448573</v>
+        <v>0.441</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2260,7 +2260,7 @@
         <v>1.3040000000000003</v>
       </c>
       <c r="D130">
-        <v>0.27887093789062983</v>
+        <v>0.27900000000000003</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -2274,7 +2274,7 @@
         <v>1.2720000000000002</v>
       </c>
       <c r="D131">
-        <v>0.20106963967740143</v>
+        <v>0.20100000000000001</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2288,7 +2288,7 @@
         <v>1.5690000000000002</v>
       </c>
       <c r="D132">
-        <v>0.74916420095997605</v>
+        <v>0.749</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2302,7 +2302,7 @@
         <v>1.1470000000000002</v>
       </c>
       <c r="D133">
-        <v>0.39736632972611047</v>
+        <v>0.39700000000000002</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -2316,7 +2316,7 @@
         <v>1.3250000000000002</v>
       </c>
       <c r="D134">
-        <v>0.34152745131248236</v>
+        <v>0.34200000000000003</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -2330,7 +2330,7 @@
         <v>1.4530000000000001</v>
       </c>
       <c r="D135">
-        <v>0.30596731851621001</v>
+        <v>0.30599999999999999</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2344,7 +2344,7 @@
         <v>1.5529999999999999</v>
       </c>
       <c r="D136">
-        <v>0.49198882101121033</v>
+        <v>0.49199999999999999</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -2358,7 +2358,7 @@
         <v>1.4039999999999999</v>
       </c>
       <c r="D137">
-        <v>0.84377011087143816</v>
+        <v>0.84399999999999997</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -2372,7 +2372,7 @@
         <v>1.871</v>
       </c>
       <c r="D138">
-        <v>0.29185098937642945</v>
+        <v>0.29199999999999998</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -2386,7 +2386,7 @@
         <v>1.4509999999999998</v>
       </c>
       <c r="D139">
-        <v>0.22518658929874011</v>
+        <v>0.22500000000000001</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -2400,7 +2400,7 @@
         <v>1.4319999999999999</v>
       </c>
       <c r="D140">
-        <v>0.23698945124203288</v>
+        <v>0.23699999999999999</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -2414,7 +2414,7 @@
         <v>1.9549999999999998</v>
       </c>
       <c r="D141">
-        <v>0.55531162422553437</v>
+        <v>0.55500000000000005</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
         <v>1.6279999999999999</v>
       </c>
       <c r="D142">
-        <v>0.39031653820969492</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -2442,7 +2442,7 @@
         <v>1.873</v>
       </c>
       <c r="D143">
-        <v>0.35406072925417692</v>
+        <v>0.35399999999999998</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
         <v>2.2920000000000003</v>
       </c>
       <c r="D144">
-        <v>0.72921670304512409</v>
+        <v>0.72899999999999998</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -2470,7 +2470,7 @@
         <v>1.7869999999999999</v>
       </c>
       <c r="D145">
-        <v>0.52266145830738209</v>
+        <v>0.52300000000000002</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -2484,7 +2484,7 @@
         <v>1.7629999999999999</v>
       </c>
       <c r="D146">
-        <v>0.2477337280226502</v>
+        <v>0.248</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -2498,7 +2498,7 @@
         <v>2.19</v>
       </c>
       <c r="D147">
-        <v>0.52795170233649291</v>
+        <v>0.52800000000000002</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -2512,7 +2512,7 @@
         <v>1.9809999999999999</v>
       </c>
       <c r="D148">
-        <v>0.26270325464295258</v>
+        <v>0.26300000000000001</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -2526,7 +2526,7 @@
         <v>2.1180000000000003</v>
       </c>
       <c r="D149">
-        <v>0.6944991000714118</v>
+        <v>0.69399999999999995</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -2540,7 +2540,7 @@
         <v>2.3810000000000002</v>
       </c>
       <c r="D150">
-        <v>0.45264666131542342</v>
+        <v>0.45300000000000001</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -2554,7 +2554,7 @@
         <v>2.3650000000000002</v>
       </c>
       <c r="D151">
-        <v>0.87467536835102455</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -2568,7 +2568,7 @@
         <v>2.6370000000000005</v>
       </c>
       <c r="D152">
-        <v>8.1853527718724242E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
         <v>2.5920000000000001</v>
       </c>
       <c r="D153">
-        <v>0.35703081099535605</v>
+        <v>0.35699999999999998</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -2596,7 +2596,7 @@
         <v>2.5640000000000005</v>
       </c>
       <c r="D154">
-        <v>0.18278129007094857</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -2610,7 +2610,7 @@
         <v>2.4680000000000004</v>
       </c>
       <c r="D155">
-        <v>6.9310893804654786E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -2624,7 +2624,7 @@
         <v>2.3890000000000002</v>
       </c>
       <c r="D156">
-        <v>0.34655302624562084</v>
+        <v>0.34699999999999998</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
         <v>2.6880000000000002</v>
       </c>
       <c r="D157">
-        <v>0.5606255434779962</v>
+        <v>0.56100000000000005</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -2652,7 +2652,7 @@
         <v>2.9649999999999999</v>
       </c>
       <c r="D158">
-        <v>0.56876269216607278</v>
+        <v>0.56899999999999995</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -2666,7 +2666,7 @@
         <v>2.6880000000000002</v>
       </c>
       <c r="D159">
-        <v>0.66122688995533085</v>
+        <v>0.66100000000000003</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -2680,7 +2680,7 @@
         <v>2.8290000000000002</v>
       </c>
       <c r="D160">
-        <v>0.69353226312840033</v>
+        <v>0.69399999999999995</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -2694,7 +2694,7 @@
         <v>2.952</v>
       </c>
       <c r="D161">
-        <v>0.72610398704317947</v>
+        <v>0.72599999999999998</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -2708,7 +2708,7 @@
         <v>3.1080000000000001</v>
       </c>
       <c r="D162">
-        <v>0.79525656237468245</v>
+        <v>0.79500000000000004</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -2722,7 +2722,7 @@
         <v>2.9740000000000002</v>
       </c>
       <c r="D163">
-        <v>0.46885818751515679</v>
+        <v>0.46899999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>